<commit_message>
Add local 2054 dataset comparison to Excel file
Updated Excel file to include comparison with local enhanced 2054 dataset,
showing significantly larger impacts than Enhanced CPS 2024 projection.

Excel now includes:
- Revenue summary with both 2054 datasets (-$176.3B vs -$588.1B)
- 2026 comparison table
- 2034 comparison table
- 2054 Enhanced CPS 2024 comparison (-$176.3B)
- 2054 Local dataset comparison (-$588.1B)

Local 2054 dataset shows much larger impacts:
- First quintile: -$312 vs -$5 Wharton (6,240% difference)
- 90-95%: -$13,974 vs -$4,385 Wharton (219% difference)
- Suggests different benefit/inflation assumptions

All tables formatted with clean style matching requested design.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/wharton_comparison_enhanced_cps_2024.xlsx
+++ b/data/wharton_comparison_enhanced_cps_2024.xlsx
@@ -84,6 +84,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -105,7 +106,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,11 @@
           <t>-$85.4B</t>
         </is>
       </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>(Enhanced CPS 2024)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -516,6 +521,11 @@
           <t>-$131.7B</t>
         </is>
       </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>(Enhanced CPS 2024)</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -528,852 +538,1152 @@
           <t>-$176.3B</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>(Enhanced CPS 2024)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Year 2054 (Local):</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>-$588.1B</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>(Local enhanced dataset)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Average Tax Change per Household (Dollars) - Year 2026</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t>Income Group</t>
-        </is>
-      </c>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>PolicyEngine</t>
-        </is>
-      </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>Wharton</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="inlineStr">
-        <is>
-          <t>Difference</t>
-        </is>
-      </c>
-      <c r="E8" s="4" t="inlineStr">
-        <is>
-          <t>% Diff</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
+          <t>Income Group</t>
+        </is>
+      </c>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>PolicyEngine</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>Wharton</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="E9" s="5" t="inlineStr">
+        <is>
+          <t>% Diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
           <t>First quintile</t>
         </is>
       </c>
-      <c r="B9" s="6" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>-$24</t>
         </is>
       </c>
-      <c r="C9" s="6" t="inlineStr">
+      <c r="C10" s="7" t="inlineStr">
         <is>
           <t>$0</t>
         </is>
       </c>
-      <c r="D9" s="6" t="inlineStr">
+      <c r="D10" s="7" t="inlineStr">
         <is>
           <t>-$24</t>
         </is>
       </c>
-      <c r="E9" s="7" t="inlineStr">
+      <c r="E10" s="8" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="8" t="inlineStr">
+    <row r="11">
+      <c r="A11" s="9" t="inlineStr">
         <is>
           <t>Second quintile</t>
         </is>
       </c>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="B11" s="10" t="inlineStr">
         <is>
           <t>-$65</t>
         </is>
       </c>
-      <c r="C10" s="9" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr">
         <is>
           <t>-$15</t>
         </is>
       </c>
-      <c r="D10" s="9" t="inlineStr">
+      <c r="D11" s="10" t="inlineStr">
         <is>
           <t>-$50</t>
         </is>
       </c>
-      <c r="E10" s="10" t="inlineStr">
+      <c r="E11" s="11" t="inlineStr">
         <is>
           <t>333%</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="5" t="inlineStr">
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
         <is>
           <t>Middle quintile</t>
         </is>
       </c>
-      <c r="B11" s="6" t="inlineStr">
+      <c r="B12" s="7" t="inlineStr">
         <is>
           <t>-$417</t>
         </is>
       </c>
-      <c r="C11" s="6" t="inlineStr">
+      <c r="C12" s="7" t="inlineStr">
         <is>
           <t>-$340</t>
         </is>
       </c>
-      <c r="D11" s="6" t="inlineStr">
+      <c r="D12" s="7" t="inlineStr">
         <is>
           <t>-$77</t>
         </is>
       </c>
-      <c r="E11" s="7" t="inlineStr">
+      <c r="E12" s="8" t="inlineStr">
         <is>
           <t>23%</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="8" t="inlineStr">
+    <row r="13">
+      <c r="A13" s="9" t="inlineStr">
         <is>
           <t>Fourth quintile</t>
         </is>
       </c>
-      <c r="B12" s="9" t="inlineStr">
+      <c r="B13" s="10" t="inlineStr">
         <is>
           <t>-$763</t>
         </is>
       </c>
-      <c r="C12" s="9" t="inlineStr">
+      <c r="C13" s="10" t="inlineStr">
         <is>
           <t>-$1,135</t>
         </is>
       </c>
-      <c r="D12" s="9" t="inlineStr">
+      <c r="D13" s="10" t="inlineStr">
         <is>
           <t>+$372</t>
         </is>
       </c>
-      <c r="E12" s="10" t="inlineStr">
+      <c r="E13" s="11" t="inlineStr">
         <is>
           <t>-33%</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="5" t="inlineStr">
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
         <is>
           <t>80-90%</t>
         </is>
       </c>
-      <c r="B13" s="6" t="inlineStr">
+      <c r="B14" s="7" t="inlineStr">
         <is>
           <t>-$2,148</t>
         </is>
       </c>
-      <c r="C13" s="6" t="inlineStr">
+      <c r="C14" s="7" t="inlineStr">
         <is>
           <t>-$1,625</t>
         </is>
       </c>
-      <c r="D13" s="6" t="inlineStr">
+      <c r="D14" s="7" t="inlineStr">
         <is>
           <t>-$523</t>
         </is>
       </c>
-      <c r="E13" s="7" t="inlineStr">
+      <c r="E14" s="8" t="inlineStr">
         <is>
           <t>32%</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="8" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="9" t="inlineStr">
         <is>
           <t>90-95%</t>
         </is>
       </c>
-      <c r="B14" s="9" t="inlineStr">
+      <c r="B15" s="10" t="inlineStr">
         <is>
           <t>-$2,907</t>
         </is>
       </c>
-      <c r="C14" s="9" t="inlineStr">
+      <c r="C15" s="10" t="inlineStr">
         <is>
           <t>-$1,590</t>
         </is>
       </c>
-      <c r="D14" s="9" t="inlineStr">
+      <c r="D15" s="10" t="inlineStr">
         <is>
           <t>-$1,317</t>
         </is>
       </c>
-      <c r="E14" s="10" t="inlineStr">
+      <c r="E15" s="11" t="inlineStr">
         <is>
           <t>83%</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="5" t="inlineStr">
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
         <is>
           <t>95-99%</t>
         </is>
       </c>
-      <c r="B15" s="6" t="inlineStr">
+      <c r="B16" s="7" t="inlineStr">
         <is>
           <t>-$1,972</t>
         </is>
       </c>
-      <c r="C15" s="6" t="inlineStr">
+      <c r="C16" s="7" t="inlineStr">
         <is>
           <t>-$2,020</t>
         </is>
       </c>
-      <c r="D15" s="6" t="inlineStr">
+      <c r="D16" s="7" t="inlineStr">
         <is>
           <t>+$48</t>
         </is>
       </c>
-      <c r="E15" s="7" t="inlineStr">
+      <c r="E16" s="8" t="inlineStr">
         <is>
           <t>-2%</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="8" t="inlineStr">
+    <row r="17">
+      <c r="A17" s="9" t="inlineStr">
         <is>
           <t>99-99.9%</t>
         </is>
       </c>
-      <c r="B16" s="9" t="inlineStr">
+      <c r="B17" s="10" t="inlineStr">
         <is>
           <t>-$1,608</t>
         </is>
       </c>
-      <c r="C16" s="9" t="inlineStr">
+      <c r="C17" s="10" t="inlineStr">
         <is>
           <t>-$2,205</t>
         </is>
       </c>
-      <c r="D16" s="9" t="inlineStr">
+      <c r="D17" s="10" t="inlineStr">
         <is>
           <t>+$597</t>
         </is>
       </c>
-      <c r="E16" s="10" t="inlineStr">
+      <c r="E17" s="11" t="inlineStr">
         <is>
           <t>-27%</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="5" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
         <is>
           <t>Top 0.1%</t>
         </is>
       </c>
-      <c r="B17" s="6" t="inlineStr">
+      <c r="B18" s="7" t="inlineStr">
         <is>
           <t>$0</t>
         </is>
       </c>
-      <c r="C17" s="6" t="inlineStr">
+      <c r="C18" s="7" t="inlineStr">
         <is>
           <t>-$2,450</t>
         </is>
       </c>
-      <c r="D17" s="6" t="inlineStr">
+      <c r="D18" s="7" t="inlineStr">
         <is>
           <t>+$2,450</t>
         </is>
       </c>
-      <c r="E17" s="7" t="inlineStr">
+      <c r="E18" s="8" t="inlineStr">
         <is>
           <t>-100%</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
         <is>
           <t>Average Tax Change per Household (Dollars) - Year 2034</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="inlineStr">
-        <is>
-          <t>Income Group</t>
-        </is>
-      </c>
-      <c r="B20" s="4" t="inlineStr">
-        <is>
-          <t>PolicyEngine</t>
-        </is>
-      </c>
-      <c r="C20" s="4" t="inlineStr">
-        <is>
-          <t>Wharton</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="inlineStr">
-        <is>
-          <t>Difference</t>
-        </is>
-      </c>
-      <c r="E20" s="4" t="inlineStr">
-        <is>
-          <t>% Diff</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="inlineStr">
         <is>
+          <t>Income Group</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>PolicyEngine</t>
+        </is>
+      </c>
+      <c r="C21" s="5" t="inlineStr">
+        <is>
+          <t>Wharton</t>
+        </is>
+      </c>
+      <c r="D21" s="5" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="E21" s="5" t="inlineStr">
+        <is>
+          <t>% Diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
           <t>First quintile</t>
         </is>
       </c>
-      <c r="B21" s="6" t="inlineStr">
+      <c r="B22" s="7" t="inlineStr">
         <is>
           <t>-$39</t>
         </is>
       </c>
-      <c r="C21" s="6" t="inlineStr">
+      <c r="C22" s="7" t="inlineStr">
         <is>
           <t>$0</t>
         </is>
       </c>
-      <c r="D21" s="6" t="inlineStr">
+      <c r="D22" s="7" t="inlineStr">
         <is>
           <t>-$39</t>
         </is>
       </c>
-      <c r="E21" s="7" t="inlineStr">
+      <c r="E22" s="8" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="8" t="inlineStr">
+    <row r="23">
+      <c r="A23" s="9" t="inlineStr">
         <is>
           <t>Second quintile</t>
         </is>
       </c>
-      <c r="B22" s="9" t="inlineStr">
+      <c r="B23" s="10" t="inlineStr">
         <is>
           <t>-$195</t>
         </is>
       </c>
-      <c r="C22" s="9" t="inlineStr">
+      <c r="C23" s="10" t="inlineStr">
         <is>
           <t>-$45</t>
         </is>
       </c>
-      <c r="D22" s="9" t="inlineStr">
+      <c r="D23" s="10" t="inlineStr">
         <is>
           <t>-$150</t>
         </is>
       </c>
-      <c r="E22" s="10" t="inlineStr">
+      <c r="E23" s="11" t="inlineStr">
         <is>
           <t>333%</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="5" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
         <is>
           <t>Middle quintile</t>
         </is>
       </c>
-      <c r="B23" s="6" t="inlineStr">
+      <c r="B24" s="7" t="inlineStr">
         <is>
           <t>-$769</t>
         </is>
       </c>
-      <c r="C23" s="6" t="inlineStr">
+      <c r="C24" s="7" t="inlineStr">
         <is>
           <t>-$615</t>
         </is>
       </c>
-      <c r="D23" s="6" t="inlineStr">
+      <c r="D24" s="7" t="inlineStr">
         <is>
           <t>-$154</t>
         </is>
       </c>
-      <c r="E23" s="7" t="inlineStr">
+      <c r="E24" s="8" t="inlineStr">
         <is>
           <t>25%</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="8" t="inlineStr">
+    <row r="25">
+      <c r="A25" s="9" t="inlineStr">
         <is>
           <t>Fourth quintile</t>
         </is>
       </c>
-      <c r="B24" s="9" t="inlineStr">
+      <c r="B25" s="10" t="inlineStr">
         <is>
           <t>-$1,291</t>
         </is>
       </c>
-      <c r="C24" s="9" t="inlineStr">
+      <c r="C25" s="10" t="inlineStr">
         <is>
           <t>-$1,630</t>
         </is>
       </c>
-      <c r="D24" s="9" t="inlineStr">
+      <c r="D25" s="10" t="inlineStr">
         <is>
           <t>+$339</t>
         </is>
       </c>
-      <c r="E24" s="10" t="inlineStr">
+      <c r="E25" s="11" t="inlineStr">
         <is>
           <t>-21%</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="5" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
         <is>
           <t>80-90%</t>
         </is>
       </c>
-      <c r="B25" s="6" t="inlineStr">
+      <c r="B26" s="7" t="inlineStr">
         <is>
           <t>-$3,053</t>
         </is>
       </c>
-      <c r="C25" s="6" t="inlineStr">
+      <c r="C26" s="7" t="inlineStr">
         <is>
           <t>-$2,160</t>
         </is>
       </c>
-      <c r="D25" s="6" t="inlineStr">
+      <c r="D26" s="7" t="inlineStr">
         <is>
           <t>-$893</t>
         </is>
       </c>
-      <c r="E25" s="7" t="inlineStr">
+      <c r="E26" s="8" t="inlineStr">
         <is>
           <t>41%</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="8" t="inlineStr">
+    <row r="27">
+      <c r="A27" s="9" t="inlineStr">
         <is>
           <t>90-95%</t>
         </is>
       </c>
-      <c r="B26" s="9" t="inlineStr">
+      <c r="B27" s="10" t="inlineStr">
         <is>
           <t>-$3,388</t>
         </is>
       </c>
-      <c r="C26" s="9" t="inlineStr">
+      <c r="C27" s="10" t="inlineStr">
         <is>
           <t>-$2,160</t>
         </is>
       </c>
-      <c r="D26" s="9" t="inlineStr">
+      <c r="D27" s="10" t="inlineStr">
         <is>
           <t>-$1,228</t>
         </is>
       </c>
-      <c r="E26" s="10" t="inlineStr">
+      <c r="E27" s="11" t="inlineStr">
         <is>
           <t>57%</t>
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="5" t="inlineStr">
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
         <is>
           <t>95-99%</t>
         </is>
       </c>
-      <c r="B27" s="6" t="inlineStr">
+      <c r="B28" s="7" t="inlineStr">
         <is>
           <t>-$2,325</t>
         </is>
       </c>
-      <c r="C27" s="6" t="inlineStr">
+      <c r="C28" s="7" t="inlineStr">
         <is>
           <t>-$2,605</t>
         </is>
       </c>
-      <c r="D27" s="6" t="inlineStr">
+      <c r="D28" s="7" t="inlineStr">
         <is>
           <t>+$280</t>
         </is>
       </c>
-      <c r="E27" s="7" t="inlineStr">
+      <c r="E28" s="8" t="inlineStr">
         <is>
           <t>-11%</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="8" t="inlineStr">
+    <row r="29">
+      <c r="A29" s="9" t="inlineStr">
         <is>
           <t>99-99.9%</t>
         </is>
       </c>
-      <c r="B28" s="9" t="inlineStr">
+      <c r="B29" s="10" t="inlineStr">
         <is>
           <t>-$2,250</t>
         </is>
       </c>
-      <c r="C28" s="9" t="inlineStr">
+      <c r="C29" s="10" t="inlineStr">
         <is>
           <t>-$2,715</t>
         </is>
       </c>
-      <c r="D28" s="9" t="inlineStr">
+      <c r="D29" s="10" t="inlineStr">
         <is>
           <t>+$465</t>
         </is>
       </c>
-      <c r="E28" s="10" t="inlineStr">
+      <c r="E29" s="11" t="inlineStr">
         <is>
           <t>-17%</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="5" t="inlineStr">
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
         <is>
           <t>Top 0.1%</t>
         </is>
       </c>
-      <c r="B29" s="6" t="inlineStr">
+      <c r="B30" s="7" t="inlineStr">
         <is>
           <t>$0</t>
         </is>
       </c>
-      <c r="C29" s="6" t="inlineStr">
+      <c r="C30" s="7" t="inlineStr">
         <is>
           <t>-$2,970</t>
         </is>
       </c>
-      <c r="D29" s="6" t="inlineStr">
+      <c r="D30" s="7" t="inlineStr">
         <is>
           <t>+$2,970</t>
         </is>
       </c>
-      <c r="E29" s="7" t="inlineStr">
+      <c r="E30" s="8" t="inlineStr">
         <is>
           <t>-100%</t>
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>Average Tax Change per Household (Dollars) - Year 2054</t>
-        </is>
-      </c>
-    </row>
     <row r="32">
-      <c r="A32" s="4" t="inlineStr">
-        <is>
-          <t>Income Group</t>
-        </is>
-      </c>
-      <c r="B32" s="4" t="inlineStr">
-        <is>
-          <t>PolicyEngine</t>
-        </is>
-      </c>
-      <c r="C32" s="4" t="inlineStr">
-        <is>
-          <t>Wharton</t>
-        </is>
-      </c>
-      <c r="D32" s="4" t="inlineStr">
-        <is>
-          <t>Difference</t>
-        </is>
-      </c>
-      <c r="E32" s="4" t="inlineStr">
-        <is>
-          <t>% Diff</t>
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>Average Tax Change per Household (Dollars) - Year 2054 (Enhanced CPS 2024)</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="inlineStr">
         <is>
+          <t>Income Group</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="inlineStr">
+        <is>
+          <t>PolicyEngine</t>
+        </is>
+      </c>
+      <c r="C33" s="5" t="inlineStr">
+        <is>
+          <t>Wharton</t>
+        </is>
+      </c>
+      <c r="D33" s="5" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="E33" s="5" t="inlineStr">
+        <is>
+          <t>% Diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
           <t>First quintile</t>
         </is>
       </c>
-      <c r="B33" s="6" t="inlineStr">
+      <c r="B34" s="7" t="inlineStr">
         <is>
           <t>-$5</t>
         </is>
       </c>
-      <c r="C33" s="6" t="inlineStr">
+      <c r="C34" s="7" t="inlineStr">
         <is>
           <t>-$5</t>
         </is>
       </c>
-      <c r="D33" s="6" t="inlineStr">
+      <c r="D34" s="7" t="inlineStr">
         <is>
           <t>$0</t>
         </is>
       </c>
-      <c r="E33" s="7" t="inlineStr">
+      <c r="E34" s="8" t="inlineStr">
         <is>
           <t>0% ✓</t>
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="8" t="inlineStr">
+    <row r="35">
+      <c r="A35" s="9" t="inlineStr">
         <is>
           <t>Second quintile</t>
         </is>
       </c>
-      <c r="B34" s="9" t="inlineStr">
+      <c r="B35" s="10" t="inlineStr">
         <is>
           <t>-$242</t>
         </is>
       </c>
-      <c r="C34" s="9" t="inlineStr">
+      <c r="C35" s="10" t="inlineStr">
         <is>
           <t>-$275</t>
         </is>
       </c>
-      <c r="D34" s="9" t="inlineStr">
+      <c r="D35" s="10" t="inlineStr">
         <is>
           <t>+$33</t>
         </is>
       </c>
-      <c r="E34" s="10" t="inlineStr">
+      <c r="E35" s="11" t="inlineStr">
         <is>
           <t>-12%</t>
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="5" t="inlineStr">
+    <row r="36">
+      <c r="A36" s="6" t="inlineStr">
         <is>
           <t>Middle quintile</t>
         </is>
       </c>
-      <c r="B35" s="6" t="inlineStr">
+      <c r="B36" s="7" t="inlineStr">
         <is>
           <t>-$757</t>
         </is>
       </c>
-      <c r="C35" s="6" t="inlineStr">
+      <c r="C36" s="7" t="inlineStr">
         <is>
           <t>-$1,730</t>
         </is>
       </c>
-      <c r="D35" s="6" t="inlineStr">
+      <c r="D36" s="7" t="inlineStr">
         <is>
           <t>+$973</t>
         </is>
       </c>
-      <c r="E35" s="7" t="inlineStr">
+      <c r="E36" s="8" t="inlineStr">
         <is>
           <t>-56%</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="8" t="inlineStr">
+    <row r="37">
+      <c r="A37" s="9" t="inlineStr">
         <is>
           <t>Fourth quintile</t>
         </is>
       </c>
-      <c r="B36" s="9" t="inlineStr">
+      <c r="B37" s="10" t="inlineStr">
         <is>
           <t>-$1,558</t>
         </is>
       </c>
-      <c r="C36" s="9" t="inlineStr">
+      <c r="C37" s="10" t="inlineStr">
         <is>
           <t>-$3,560</t>
         </is>
       </c>
-      <c r="D36" s="9" t="inlineStr">
+      <c r="D37" s="10" t="inlineStr">
         <is>
           <t>+$2,002</t>
         </is>
       </c>
-      <c r="E36" s="10" t="inlineStr">
+      <c r="E37" s="11" t="inlineStr">
         <is>
           <t>-56%</t>
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="5" t="inlineStr">
+    <row r="38">
+      <c r="A38" s="6" t="inlineStr">
         <is>
           <t>80-90%</t>
         </is>
       </c>
-      <c r="B37" s="6" t="inlineStr">
+      <c r="B38" s="7" t="inlineStr">
         <is>
           <t>-$3,518</t>
         </is>
       </c>
-      <c r="C37" s="6" t="inlineStr">
+      <c r="C38" s="7" t="inlineStr">
         <is>
           <t>-$4,075</t>
         </is>
       </c>
-      <c r="D37" s="6" t="inlineStr">
+      <c r="D38" s="7" t="inlineStr">
         <is>
           <t>+$557</t>
         </is>
       </c>
-      <c r="E37" s="7" t="inlineStr">
+      <c r="E38" s="8" t="inlineStr">
         <is>
           <t>-14%</t>
         </is>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="8" t="inlineStr">
+    <row r="39">
+      <c r="A39" s="9" t="inlineStr">
         <is>
           <t>90-95%</t>
         </is>
       </c>
-      <c r="B38" s="9" t="inlineStr">
+      <c r="B39" s="10" t="inlineStr">
         <is>
           <t>-$5,094</t>
         </is>
       </c>
-      <c r="C38" s="9" t="inlineStr">
+      <c r="C39" s="10" t="inlineStr">
         <is>
           <t>-$4,385</t>
         </is>
       </c>
-      <c r="D38" s="9" t="inlineStr">
+      <c r="D39" s="10" t="inlineStr">
         <is>
           <t>-$709</t>
         </is>
       </c>
-      <c r="E38" s="10" t="inlineStr">
+      <c r="E39" s="11" t="inlineStr">
         <is>
           <t>16%</t>
         </is>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="5" t="inlineStr">
+    <row r="40">
+      <c r="A40" s="6" t="inlineStr">
         <is>
           <t>95-99%</t>
         </is>
       </c>
-      <c r="B39" s="6" t="inlineStr">
+      <c r="B40" s="7" t="inlineStr">
         <is>
           <t>-$5,183</t>
         </is>
       </c>
-      <c r="C39" s="6" t="inlineStr">
+      <c r="C40" s="7" t="inlineStr">
         <is>
           <t>-$4,565</t>
         </is>
       </c>
-      <c r="D39" s="6" t="inlineStr">
+      <c r="D40" s="7" t="inlineStr">
         <is>
           <t>-$618</t>
         </is>
       </c>
-      <c r="E39" s="7" t="inlineStr">
+      <c r="E40" s="8" t="inlineStr">
         <is>
           <t>14%</t>
         </is>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="8" t="inlineStr">
+    <row r="41">
+      <c r="A41" s="9" t="inlineStr">
         <is>
           <t>99-99.9%</t>
         </is>
       </c>
-      <c r="B40" s="9" t="inlineStr">
+      <c r="B41" s="10" t="inlineStr">
         <is>
           <t>-$3,231</t>
         </is>
       </c>
-      <c r="C40" s="9" t="inlineStr">
+      <c r="C41" s="10" t="inlineStr">
         <is>
           <t>-$4,820</t>
         </is>
       </c>
-      <c r="D40" s="9" t="inlineStr">
+      <c r="D41" s="10" t="inlineStr">
         <is>
           <t>+$1,589</t>
         </is>
       </c>
-      <c r="E40" s="10" t="inlineStr">
+      <c r="E41" s="11" t="inlineStr">
         <is>
           <t>-33%</t>
         </is>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="5" t="inlineStr">
+    <row r="42">
+      <c r="A42" s="6" t="inlineStr">
         <is>
           <t>Top 0.1%</t>
         </is>
       </c>
-      <c r="B41" s="6" t="inlineStr">
+      <c r="B42" s="7" t="inlineStr">
         <is>
           <t>$0</t>
         </is>
       </c>
-      <c r="C41" s="6" t="inlineStr">
+      <c r="C42" s="7" t="inlineStr">
         <is>
           <t>-$5,080</t>
         </is>
       </c>
-      <c r="D41" s="6" t="inlineStr">
+      <c r="D42" s="7" t="inlineStr">
         <is>
           <t>+$5,080</t>
         </is>
       </c>
-      <c r="E41" s="7" t="inlineStr">
+      <c r="E42" s="8" t="inlineStr">
         <is>
           <t>-100%</t>
         </is>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="11" t="inlineStr">
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>Average Tax Change per Household (Dollars) - Year 2054 (Local Enhanced Dataset)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="5" t="inlineStr">
+        <is>
+          <t>Income Group</t>
+        </is>
+      </c>
+      <c r="B45" s="5" t="inlineStr">
+        <is>
+          <t>PolicyEngine</t>
+        </is>
+      </c>
+      <c r="C45" s="5" t="inlineStr">
+        <is>
+          <t>Wharton</t>
+        </is>
+      </c>
+      <c r="D45" s="5" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="E45" s="5" t="inlineStr">
+        <is>
+          <t>% Diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="inlineStr">
+        <is>
+          <t>First quintile</t>
+        </is>
+      </c>
+      <c r="B46" s="7" t="inlineStr">
+        <is>
+          <t>-$312</t>
+        </is>
+      </c>
+      <c r="C46" s="7" t="inlineStr">
+        <is>
+          <t>-$5</t>
+        </is>
+      </c>
+      <c r="D46" s="7" t="inlineStr">
+        <is>
+          <t>-$307</t>
+        </is>
+      </c>
+      <c r="E46" s="8" t="inlineStr">
+        <is>
+          <t>6240%</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="9" t="inlineStr">
+        <is>
+          <t>Second quintile</t>
+        </is>
+      </c>
+      <c r="B47" s="10" t="inlineStr">
+        <is>
+          <t>-$1,119</t>
+        </is>
+      </c>
+      <c r="C47" s="10" t="inlineStr">
+        <is>
+          <t>-$275</t>
+        </is>
+      </c>
+      <c r="D47" s="10" t="inlineStr">
+        <is>
+          <t>-$844</t>
+        </is>
+      </c>
+      <c r="E47" s="11" t="inlineStr">
+        <is>
+          <t>307%</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="6" t="inlineStr">
+        <is>
+          <t>Middle quintile</t>
+        </is>
+      </c>
+      <c r="B48" s="7" t="inlineStr">
+        <is>
+          <t>-$2,982</t>
+        </is>
+      </c>
+      <c r="C48" s="7" t="inlineStr">
+        <is>
+          <t>-$1,730</t>
+        </is>
+      </c>
+      <c r="D48" s="7" t="inlineStr">
+        <is>
+          <t>-$1,252</t>
+        </is>
+      </c>
+      <c r="E48" s="8" t="inlineStr">
+        <is>
+          <t>72%</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="9" t="inlineStr">
+        <is>
+          <t>Fourth quintile</t>
+        </is>
+      </c>
+      <c r="B49" s="10" t="inlineStr">
+        <is>
+          <t>-$4,342</t>
+        </is>
+      </c>
+      <c r="C49" s="10" t="inlineStr">
+        <is>
+          <t>-$3,560</t>
+        </is>
+      </c>
+      <c r="D49" s="10" t="inlineStr">
+        <is>
+          <t>-$782</t>
+        </is>
+      </c>
+      <c r="E49" s="11" t="inlineStr">
+        <is>
+          <t>22%</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="6" t="inlineStr">
+        <is>
+          <t>80-90%</t>
+        </is>
+      </c>
+      <c r="B50" s="7" t="inlineStr">
+        <is>
+          <t>-$9,064</t>
+        </is>
+      </c>
+      <c r="C50" s="7" t="inlineStr">
+        <is>
+          <t>-$4,075</t>
+        </is>
+      </c>
+      <c r="D50" s="7" t="inlineStr">
+        <is>
+          <t>-$4,989</t>
+        </is>
+      </c>
+      <c r="E50" s="8" t="inlineStr">
+        <is>
+          <t>122%</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="9" t="inlineStr">
+        <is>
+          <t>90-95%</t>
+        </is>
+      </c>
+      <c r="B51" s="10" t="inlineStr">
+        <is>
+          <t>-$13,974</t>
+        </is>
+      </c>
+      <c r="C51" s="10" t="inlineStr">
+        <is>
+          <t>-$4,385</t>
+        </is>
+      </c>
+      <c r="D51" s="10" t="inlineStr">
+        <is>
+          <t>-$9,589</t>
+        </is>
+      </c>
+      <c r="E51" s="11" t="inlineStr">
+        <is>
+          <t>219%</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6" t="inlineStr">
+        <is>
+          <t>95-99%</t>
+        </is>
+      </c>
+      <c r="B52" s="7" t="inlineStr">
+        <is>
+          <t>-$6,113</t>
+        </is>
+      </c>
+      <c r="C52" s="7" t="inlineStr">
+        <is>
+          <t>-$4,565</t>
+        </is>
+      </c>
+      <c r="D52" s="7" t="inlineStr">
+        <is>
+          <t>-$1,548</t>
+        </is>
+      </c>
+      <c r="E52" s="8" t="inlineStr">
+        <is>
+          <t>34%</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="9" t="inlineStr">
+        <is>
+          <t>99-99.9%</t>
+        </is>
+      </c>
+      <c r="B53" s="10" t="inlineStr">
+        <is>
+          <t>-$6,406</t>
+        </is>
+      </c>
+      <c r="C53" s="10" t="inlineStr">
+        <is>
+          <t>-$4,820</t>
+        </is>
+      </c>
+      <c r="D53" s="10" t="inlineStr">
+        <is>
+          <t>-$1,586</t>
+        </is>
+      </c>
+      <c r="E53" s="11" t="inlineStr">
+        <is>
+          <t>33%</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="6" t="inlineStr">
+        <is>
+          <t>Top 0.1%</t>
+        </is>
+      </c>
+      <c r="B54" s="7" t="inlineStr">
+        <is>
+          <t>-$280</t>
+        </is>
+      </c>
+      <c r="C54" s="7" t="inlineStr">
+        <is>
+          <t>-$5,080</t>
+        </is>
+      </c>
+      <c r="D54" s="7" t="inlineStr">
+        <is>
+          <t>+$4,800</t>
+        </is>
+      </c>
+      <c r="E54" s="8" t="inlineStr">
+        <is>
+          <t>-94%</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="inlineStr">
         <is>
           <t>Dataset: Enhanced CPS 2024 (reweighted to target years)</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A19:E19"/>
+  <mergeCells count="6">
+    <mergeCell ref="A20:E20"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A56:E56"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>